<commit_message>
Lab 77 RT finished
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b566d95faa460c8a/GitHub/Labs/Radiotechnics_Labs/6_sem/Lab77/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab77\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{D152FF37-9507-4AA5-8EA9-7B94F2F01B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{55489B84-1DFC-43F5-A51E-E6FBC6EC9BE7}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{D152FF37-9507-4AA5-8EA9-7B94F2F01B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9FB8E4A9-EB6B-4AC0-B6D3-7A9980BF707F}"/>
   <bookViews>
-    <workbookView xWindow="2798" yWindow="1328" windowWidth="17512" windowHeight="13597" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
+    <workbookView xWindow="4703" yWindow="900" windowWidth="17512" windowHeight="13597" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Uin</t>
   </si>
@@ -76,6 +76,42 @@
   </si>
   <si>
     <t>fгран_рас</t>
+  </si>
+  <si>
+    <t>Задание 14</t>
+  </si>
+  <si>
+    <t>Uref</t>
+  </si>
+  <si>
+    <t>Uпор</t>
+  </si>
+  <si>
+    <t>fпор</t>
+  </si>
+  <si>
+    <t>Задание 15</t>
+  </si>
+  <si>
+    <t>Uout1</t>
+  </si>
+  <si>
+    <t>Uout2</t>
+  </si>
+  <si>
+    <t>dTout</t>
+  </si>
+  <si>
+    <t>dTout1</t>
+  </si>
+  <si>
+    <t>dTout2</t>
+  </si>
+  <si>
+    <t>мс</t>
+  </si>
+  <si>
+    <t>МГц</t>
   </si>
 </sst>
 </file>
@@ -92,15 +128,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -108,12 +162,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -136,15 +291,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>323866</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57158</xdr:rowOff>
+      <xdr:colOff>338154</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171458</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -167,7 +322,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3900487" y="2362200"/>
+          <a:off x="3914775" y="2147888"/>
           <a:ext cx="2252679" cy="1133483"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -477,265 +632,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD7CE3E-4744-4BB4-B8F9-AFB388B5FA63}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E3">
         <v>1.5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I3">
         <f>E3/(G3)</f>
         <v>1.3513513513513513</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="6">
         <f>I3*100</f>
         <v>135.13513513513513</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4">
         <v>3.65</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G4">
         <v>280</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I4">
         <f>E4/(G4/100)</f>
         <v>1.3035714285714286</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f t="shared" ref="J4:J6" si="0">I4*100</f>
         <v>130.35714285714286</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E5">
         <v>3.75</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G5">
         <v>30.6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I5">
         <f>E5/(G5/100)</f>
         <v>12.254901960784315</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <f t="shared" si="0"/>
         <v>1225.4901960784314</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>3.65</v>
       </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9">
         <v>3.5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="9">
         <f>E6/(G6/100)</f>
         <v>104.28571428571428</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="10">
         <f t="shared" si="0"/>
         <v>10428.571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="12">
         <v>0.124</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B10">
         <v>12.3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <f>B10/B8</f>
         <v>99.193548387096783</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>15.7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="12">
         <v>1.86</v>
       </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="12">
         <v>4.8</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="9">
         <v>0.50600000000000001</v>
       </c>
-      <c r="C15" t="s">
-        <v>3</v>
+      <c r="C15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="9">
+        <v>18</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="12">
+        <v>22.1</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1.32</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="12">
+        <f>1/E20</f>
+        <v>0.75757575757575757</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>216</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>1.306</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G22" si="1">1/E21</f>
+        <v>0.76569678407350683</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9">
+        <v>240</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>0.76161462300076166</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lab 6101 is almost finished
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab77\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{D152FF37-9507-4AA5-8EA9-7B94F2F01B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9FB8E4A9-EB6B-4AC0-B6D3-7A9980BF707F}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{D152FF37-9507-4AA5-8EA9-7B94F2F01B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B71C2468-BFC3-42FE-9236-02D8CAE46F3A}"/>
   <bookViews>
     <workbookView xWindow="4703" yWindow="900" windowWidth="17512" windowHeight="13597" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t>Uin</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>МГц</t>
+  </si>
+  <si>
+    <t>С</t>
+  </si>
+  <si>
+    <t>мкФ</t>
   </si>
 </sst>
 </file>
@@ -154,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -242,11 +248,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -269,6 +312,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -632,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD7CE3E-4744-4BB4-B8F9-AFB388B5FA63}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -943,84 +989,187 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="23">
+        <v>0.33</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B21" s="12">
         <v>22.1</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C21" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E21" s="12">
         <v>1.32</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="12">
-        <f>1/E20</f>
+      <c r="G21" s="12">
+        <f>1/E21</f>
         <v>0.75757575757575757</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H21" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>216</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>1.306</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G21">
-        <f t="shared" ref="G21:G22" si="1">1/E21</f>
+      <c r="G22">
+        <f t="shared" ref="G22:G23" si="1">1/E22</f>
         <v>0.76569678407350683</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="16" t="s">
+    <row r="23" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B23" s="9">
         <v>240</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E23" s="9">
         <v>1.3129999999999999</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G23" s="9">
         <f t="shared" si="1"/>
         <v>0.76161462300076166</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H23" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="23">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="12">
+        <v>24.9</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="12">
+        <f>1/E25</f>
+        <v>0.81632653061224481</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>267</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G27" si="2">1/E26</f>
+        <v>0.83963056255247692</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1834</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0887316276537833</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RT Lab 77 done, Lab1 report on SSE Labs done.
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab77\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ирина Калимова\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{D152FF37-9507-4AA5-8EA9-7B94F2F01B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B71C2468-BFC3-42FE-9236-02D8CAE46F3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D88A068-8963-47B3-AEF3-DAF5385CC3D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4703" yWindow="900" windowWidth="17512" windowHeight="13597" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t>Uin</t>
   </si>
@@ -63,9 +57,6 @@
     <t>мВ</t>
   </si>
   <si>
-    <t>Усил</t>
-  </si>
-  <si>
     <t>fверх</t>
   </si>
   <si>
@@ -118,6 +109,27 @@
   </si>
   <si>
     <t>мкФ</t>
+  </si>
+  <si>
+    <t>Ko=100</t>
+  </si>
+  <si>
+    <t>Ko</t>
+  </si>
+  <si>
+    <t>20 DB/dec</t>
+  </si>
+  <si>
+    <t>dT</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>Uпор=</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -332,6 +344,903 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.670603674540682E-2"/>
+          <c:y val="8.8379629629629614E-2"/>
+          <c:w val="0.88084251968503935"/>
+          <c:h val="0.80422098279381748"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.19088809074304308"/>
+                  <c:y val="2.203816218474421E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$M$3:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.1307682802690238</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1151348331142557</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0883098412461392</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.018224820106199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F64-4DA9-9DA0-8CF5C0696778}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="180600031"/>
+        <c:axId val="74302927"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180600031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74302927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74302927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180600031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -376,6 +1285,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0D8A26-6757-4554-A121-1AF4C8A9C12E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -678,20 +1623,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD7CE3E-4744-4BB4-B8F9-AFB388B5FA63}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -711,7 +1656,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -744,8 +1689,19 @@
         <f>I3*100</f>
         <v>135.13513513513513</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <f>LOG10(C3*1000)</f>
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <f>LOG10(J3)</f>
+        <v>2.1307682802690238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -771,15 +1727,23 @@
         <v>9</v>
       </c>
       <c r="I4">
-        <f>E4/(G4/100)</f>
-        <v>1.3035714285714286</v>
+        <f>E4/(G4/1000)</f>
+        <v>13.035714285714285</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" ref="J4:J6" si="0">I4*100</f>
-        <v>130.35714285714286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1303.5714285714284</v>
+      </c>
+      <c r="L4">
+        <f>LOG10(C4*1000)</f>
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="1">LOG10(J4)</f>
+        <v>3.1151348331142557</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -805,15 +1769,23 @@
         <v>9</v>
       </c>
       <c r="I5">
-        <f>E5/(G5/100)</f>
-        <v>12.254901960784315</v>
+        <f t="shared" ref="I5:I6" si="2">E5/(G5/1000)</f>
+        <v>122.54901960784314</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="0"/>
-        <v>1225.4901960784314</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>12254.901960784313</v>
+      </c>
+      <c r="L5">
+        <f>LOG10(C5)</f>
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>4.0883098412461392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -838,21 +1810,29 @@
       <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="9">
-        <f>E6/(G6/100)</f>
-        <v>104.28571428571428</v>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1042.8571428571429</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="0"/>
-        <v>10428.571428571428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>104285.71428571429</v>
+      </c>
+      <c r="L6">
+        <f>LOG10(C6)</f>
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>5.018224820106199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
@@ -863,7 +1843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
@@ -874,7 +1854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -885,19 +1865,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <f>B10/B8</f>
         <v>99.193548387096783</v>
       </c>
       <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="9">
         <v>15.7</v>
@@ -906,12 +1889,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
@@ -922,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="12">
         <v>4.8</v>
@@ -930,10 +1913,19 @@
       <c r="F14" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>4.82</v>
+      </c>
+      <c r="M14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9">
         <v>0.50600000000000001</v>
@@ -945,14 +1937,14 @@
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="B17" s="12">
         <v>0</v>
@@ -963,10 +1955,16 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="9">
         <v>0.15</v>
@@ -975,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="9">
         <v>18</v>
@@ -983,26 +1981,35 @@
       <c r="F18" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="23">
         <v>0.33</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="12">
         <v>22.1</v>
@@ -1011,25 +2018,34 @@
         <v>3</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="12">
         <v>1.32</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G21" s="12">
         <f>1/E21</f>
         <v>0.75757575757575757</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21">
+        <v>1.32</v>
+      </c>
+      <c r="M21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>216</v>
@@ -1038,25 +2054,25 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22">
         <v>1.306</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G23" si="3">1/E22</f>
+        <v>0.76569678407350683</v>
+      </c>
+      <c r="H22" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:G23" si="1">1/E22</f>
-        <v>0.76569678407350683</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="9">
         <v>240</v>
@@ -1065,36 +2081,36 @@
         <v>9</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="9">
         <v>1.3129999999999999</v>
       </c>
       <c r="F23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="3"/>
+        <v>0.76161462300076166</v>
+      </c>
+      <c r="H23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="9">
-        <f t="shared" si="1"/>
-        <v>0.76161462300076166</v>
-      </c>
-      <c r="H23" s="17" t="s">
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="22" t="s">
-        <v>27</v>
       </c>
       <c r="B24" s="23">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="12">
         <v>24.9</v>
@@ -1103,25 +2119,34 @@
         <v>3</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" s="12">
         <v>1.2250000000000001</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="12">
         <f>1/E25</f>
         <v>0.81632653061224481</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="M25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26">
         <v>267</v>
@@ -1130,25 +2155,25 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>1.1910000000000001</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G27" si="4">1/E26</f>
+        <v>0.83963056255247692</v>
+      </c>
+      <c r="H26" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G26">
-        <f t="shared" ref="G26:G27" si="2">1/E26</f>
-        <v>0.83963056255247692</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="9">
         <v>1834</v>
@@ -1157,20 +2182,20 @@
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="9">
         <v>0.91849999999999998</v>
       </c>
       <c r="F27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="4"/>
+        <v>1.0887316276537833</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="G27" s="9">
-        <f t="shared" si="2"/>
-        <v>1.0887316276537833</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RT lab 77 added, SST lab 1 added, CM lab 5 initiated
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab77/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ирина Калимова\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab77\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D88A068-8963-47B3-AEF3-DAF5385CC3D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{0D88A068-8963-47B3-AEF3-DAF5385CC3D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{CBC9BD81-92B7-41FE-A1B2-399DB8AD1F76}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{478C2B25-9C37-4D86-BEED-F3EAE75C4BE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
   <si>
     <t>Uin</t>
   </si>
@@ -111,9 +119,6 @@
     <t>мкФ</t>
   </si>
   <si>
-    <t>Ko=100</t>
-  </si>
-  <si>
     <t>Ko</t>
   </si>
   <si>
@@ -130,6 +135,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>A(f)</t>
   </si>
 </sst>
 </file>
@@ -301,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -327,6 +335,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -530,6 +540,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>f</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36151280448315998"/>
+              <c:y val="0.86371639923441268"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -592,6 +666,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>A(f)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0253911653813574E-2"/>
+              <c:y val="0.43434343861781272"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1290,15 +1427,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>304799</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:rowOff>180022</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1321,6 +1458,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19073</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>100021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{803DC172-706B-4E92-B73C-0291F83C6AED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11672887" y="190501"/>
+          <a:ext cx="3243286" cy="1004895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1625,18 +1806,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD7CE3E-4744-4BB4-B8F9-AFB388B5FA63}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1654,34 +1835,36 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="26">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="26">
         <v>1.5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="26">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="26">
         <f>E3/(G3)</f>
         <v>1.3513513513513513</v>
       </c>
@@ -1690,7 +1873,7 @@
         <v>135.13513513513513</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3">
         <f>LOG10(C3*1000)</f>
@@ -1701,32 +1884,32 @@
         <v>2.1307682802690238</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="26">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="26">
         <v>3.65</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="26">
         <v>280</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="26">
         <f>E4/(G4/1000)</f>
         <v>13.035714285714285</v>
       </c>
@@ -1743,32 +1926,32 @@
         <v>3.1151348331142557</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="26">
         <v>100</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="26">
         <v>3.75</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="26">
         <v>30.6</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="26">
         <f t="shared" ref="I5:I6" si="2">E5/(G5/1000)</f>
         <v>122.54901960784314</v>
       </c>
@@ -1785,7 +1968,7 @@
         <v>4.0883098412461392</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -1810,7 +1993,7 @@
       <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="9">
         <f t="shared" si="2"/>
         <v>1042.8571428571429</v>
       </c>
@@ -1827,12 +2010,12 @@
         <v>5.018224820106199</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +2026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
@@ -1854,7 +2037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1865,9 +2048,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <f>B10/B8</f>
@@ -1877,8 +2060,11 @@
       <c r="K11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -1889,12 +2075,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="16" t="s">
         <v>12</v>
       </c>
@@ -1937,12 +2123,12 @@
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
@@ -1956,13 +2142,13 @@
       <c r="E17" s="12"/>
       <c r="F17" s="20"/>
       <c r="K17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L17">
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
@@ -1982,21 +2168,21 @@
         <v>4</v>
       </c>
       <c r="K18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L18">
         <v>0.14799999999999999</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
@@ -2007,7 +2193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +2220,7 @@
         <v>25</v>
       </c>
       <c r="K21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L21">
         <v>1.32</v>
@@ -2043,7 +2229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="16" t="s">
         <v>20</v>
       </c>
@@ -2097,7 +2283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="22" t="s">
         <v>26</v>
       </c>
@@ -2108,7 +2294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>12</v>
       </c>
@@ -2135,7 +2321,7 @@
         <v>25</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25">
         <v>0.13100000000000001</v>
@@ -2144,7 +2330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
         <v>19</v>
       </c>
@@ -2171,7 +2357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="16" t="s">
         <v>20</v>
       </c>

</xml_diff>